<commit_message>
Cambios Normalizacion y CuadroDeClaves
</commit_message>
<xml_diff>
--- a/documentacion-Ecommerce/CuadroDeClaves-Ecommerce.xlsx
+++ b/documentacion-Ecommerce/CuadroDeClaves-Ecommerce.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>TABLAS</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>idContado</t>
+  </si>
+  <si>
+    <t>Deposito</t>
+  </si>
+  <si>
+    <t>idDeposito</t>
   </si>
 </sst>
 </file>
@@ -596,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:E24"/>
+  <dimension ref="B2:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -692,71 +698,71 @@
     </row>
     <row r="9" spans="2:5" ht="16.5" thickBot="1">
       <c r="B9" s="11" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="2:5" ht="16.5" thickBot="1">
       <c r="B10" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="2:5" ht="16.5" thickBot="1">
       <c r="B11" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="2:5" ht="16.5" thickBot="1">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="2:5" ht="16.5" thickBot="1">
+      <c r="B13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C13" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="B13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="11" t="s">
-        <v>33</v>
-      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="11" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>28</v>
@@ -768,93 +774,105 @@
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C17" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="9" t="s">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C18" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E18" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="11" t="s">
+    <row r="19" spans="2:5">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="9" t="s">
+    <row r="20" spans="2:5">
+      <c r="B20" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C20" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10" t="s">
+      <c r="D20" s="9"/>
+      <c r="E20" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="2"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="7" t="s">
+    <row r="21" spans="2:5">
+      <c r="B21" s="2"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="10" t="s">
+    <row r="22" spans="2:5">
+      <c r="B22" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C22" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10" t="s">
+      <c r="D22" s="9"/>
+      <c r="E22" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="11" t="s">
+    <row r="23" spans="2:5">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B23" s="10" t="s">
+    <row r="24" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B24" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C24" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="10" t="s">
+      <c r="D24" s="9"/>
+      <c r="E24" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="15" customHeight="1">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="11" t="s">
+    <row r="25" spans="2:5" ht="15" customHeight="1">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="11" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
actualización de documentación de historial de carrito
Co-Authored-By: Nicolás Troche <81367277+NicolasTroche@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/documentacion-Ecommerce/CuadroDeClaves-Ecommerce.xlsx
+++ b/documentacion-Ecommerce/CuadroDeClaves-Ecommerce.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
   <si>
     <t xml:space="preserve">TABLAS</t>
   </si>
@@ -139,22 +139,40 @@
     <t xml:space="preserve">idMarca  → Marca </t>
   </si>
   <si>
+    <t xml:space="preserve">Carrito </t>
+  </si>
+  <si>
+    <t xml:space="preserve">idCarrito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idCarrito → Usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HistorialCarrito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idHistorialCarrito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IdVenta → Venta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">idCarrito → Carrito</t>
+  </si>
+  <si>
     <t xml:space="preserve">Venta</t>
   </si>
   <si>
     <t xml:space="preserve">idVenta</t>
   </si>
   <si>
-    <t xml:space="preserve">Carrito</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idUsuario + IdProducto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idUsuario → Usuario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Producto-Categoria</t>
+    <t xml:space="preserve">CarritoProducto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idCarrito + IdProducto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProductoCategoria</t>
   </si>
   <si>
     <t xml:space="preserve">idProducto + IdCategoria</t>
@@ -163,7 +181,7 @@
     <t xml:space="preserve">idCategoria → Categoria</t>
   </si>
   <si>
-    <t xml:space="preserve">Producto-Oferta</t>
+    <t xml:space="preserve">ProductoOferta</t>
   </si>
   <si>
     <t xml:space="preserve">idProducto + IdOferta</t>
@@ -179,7 +197,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -216,12 +234,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -306,39 +318,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -354,216 +366,322 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:E27"/>
+  <dimension ref="B2:E31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="48.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="48.86"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2" t="s">
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="6" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="2" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="2" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="2" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="2" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="2" t="s">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="2" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="2"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="2"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="7" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="2" t="s">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2" t="s">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="2" t="s">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2" t="s">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="8" t="s">
         <v>36</v>
       </c>
@@ -571,86 +689,126 @@
         <v>37</v>
       </c>
       <c r="D19" s="8"/>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2" t="s">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="2" t="s">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="9" t="s">
+      <c r="B22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9" t="s">
+      <c r="C22" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2" t="s">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C25" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2" t="s">
-        <v>49</v>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>